<commit_message>
fix(import): handle empty date values in import
</commit_message>
<xml_diff>
--- a/public/templates/customer-billing-template-import.xlsx
+++ b/public/templates/customer-billing-template-import.xlsx
@@ -10,17 +10,17 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t xml:space="preserve">no_kontrak</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">os_awal</t>
   </si>
   <si>
-    <t xml:space="preserve">sisa_margin</t>
+    <t xml:space="preserve">margin_sisa</t>
   </si>
   <si>
     <t xml:space="preserve">angsuran</t>
@@ -68,6 +68,39 @@
   </si>
   <si>
     <t xml:space="preserve">keterangan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tulisan berwarna merah wajib di isi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestIbu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP Cicalengka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panenjoan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cicalengka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-10-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestIbu2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-11-2024</t>
   </si>
 </sst>
 </file>
@@ -77,12 +110,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -103,14 +135,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
-      <name val="arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="arial"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -163,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,10 +202,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,180 +388,187 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1048576"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="8" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.28"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1"/>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1234567891</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>987654321</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>812345678</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>9000000</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>500000</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>500000</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1234567892</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>987654322</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>8123456782</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>9000000</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>500000</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>500000</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="1"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>